<commit_message>
Add functionality for processing materials and norms, update internal comments insertion, and refine Excel handling
</commit_message>
<xml_diff>
--- a/planilhas/planilhaPadrao.xlsx
+++ b/planilhas/planilhaPadrao.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cristopher.eichstadt\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Engenharias\Suporte Engenharias\Apoio Técnico\1. Cadastros Técnicos\Códigos_Python\Automacao\planilhas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A1082DB-C16F-409C-A5B5-1194645E1752}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6728B3E4-3A3A-4F49-AE07-55DC59B3FA27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{7E57893A-0C62-4D56-958A-83A5D7ED741F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{7E57893A-0C62-4D56-958A-83A5D7ED741F}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>item(table) + it-codigo(field)</t>
   </si>
@@ -44,54 +44,24 @@
     <t>SAP1</t>
   </si>
   <si>
-    <t>Spalte1</t>
-  </si>
-  <si>
     <t>SAP2</t>
   </si>
   <si>
-    <t>Coluna2</t>
-  </si>
-  <si>
     <t>SAP3</t>
   </si>
   <si>
-    <t>Coluna3</t>
-  </si>
-  <si>
-    <t>Coluna34</t>
-  </si>
-  <si>
     <t>Coluna32</t>
   </si>
   <si>
-    <t>Coluna33</t>
-  </si>
-  <si>
-    <t>SAP42</t>
-  </si>
-  <si>
     <t>SAP5</t>
   </si>
   <si>
     <t>SAP6</t>
   </si>
   <si>
-    <t>SAP7</t>
-  </si>
-  <si>
-    <t>SAP8</t>
-  </si>
-  <si>
-    <t>SAP9</t>
-  </si>
-  <si>
     <t>SAP10</t>
   </si>
   <si>
-    <t>SAP11</t>
-  </si>
-  <si>
     <t>SAP123</t>
   </si>
   <si>
@@ -113,43 +83,22 @@
     <t>MAKTX (PT)</t>
   </si>
   <si>
-    <t>&lt;- Length</t>
-  </si>
-  <si>
     <t>MAKTX (EN)</t>
   </si>
   <si>
     <t>MAKTX (ES)</t>
   </si>
   <si>
-    <t>MAKTX (DE) NEW</t>
-  </si>
-  <si>
     <t>MAKTX (DE)</t>
   </si>
   <si>
-    <t>ZZ_DICT_KEY_MAIN</t>
-  </si>
-  <si>
     <t>MEINS</t>
   </si>
   <si>
     <t>Product group</t>
   </si>
   <si>
-    <t>PRDHA</t>
-  </si>
-  <si>
-    <t>NTGEW + BRGEW</t>
-  </si>
-  <si>
-    <t>GEWEI</t>
-  </si>
-  <si>
     <t>MSTAE (X-Plant Mat.Status)</t>
-  </si>
-  <si>
-    <t>MSTDE (Valid from)</t>
   </si>
   <si>
     <t>Internal comment (narrative)</t>
@@ -171,7 +120,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -187,8 +136,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -225,8 +190,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor theme="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor theme="0" tint="-0.34998626667073579"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -249,38 +226,142 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -616,181 +697,132 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C0750E4-4F49-46E5-A312-5676578DE4FF}">
-  <dimension ref="A1:W2"/>
+  <dimension ref="A1:W14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="25.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="26.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="22.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="26.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="27.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7" style="13" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="25.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="26.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="22.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="26.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:23" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="2" t="s">
+      <c r="S1" s="6"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
+    </row>
+    <row r="2" spans="1:23" s="10" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="B2" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="F2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="G2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="H2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="2" t="s">
+      <c r="I2" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="4" t="s">
+      <c r="J2" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="4" t="s">
-        <v>22</v>
-      </c>
+      <c r="S2" s="11"/>
+      <c r="U2" s="12"/>
+      <c r="V2" s="11"/>
+      <c r="W2" s="11"/>
     </row>
-    <row r="2" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="S2" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="U2" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="V2" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="W2" s="5" t="s">
-        <v>42</v>
-      </c>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="K14" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>